<commit_message>
Update Test Cases table
Signed-off-by: MCBerberov19 <MCBerberov19@codingburgas.bg>
</commit_message>
<xml_diff>
--- a/docs/Test Cases.xlsx
+++ b/docs/Test Cases.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2122-10-biology-KSChervenkov19\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2122-10-biology-KSChervenkov19\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276C21A4-B36D-4B77-A449-C326D9C399F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FBF0C9-AEC0-4B8C-A372-D42D708511B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="841" xr2:uid="{D96EB1AC-1A23-4874-8F12-F051FA81C7C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="841" activeTab="1" xr2:uid="{D96EB1AC-1A23-4874-8F12-F051FA81C7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="SS-read-write-data-json" sheetId="1" r:id="rId1"/>
-    <sheet name="Values for status dropdown" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="SS-degree-utils" sheetId="3" r:id="rId2"/>
+    <sheet name="Values for status dropdown" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="57">
   <si>
     <t>Test case 1</t>
   </si>
@@ -116,15 +117,9 @@
     <t>MCBerberov19</t>
   </si>
   <si>
-    <t>07/04/2021 07:52 PM</t>
-  </si>
-  <si>
     <t>It returns a proper array data from the .json file</t>
   </si>
   <si>
-    <t>08/04/2021 02:41 PM</t>
-  </si>
-  <si>
     <t>Test Suite 1 - Automated testing of functions read/write json file data</t>
   </si>
   <si>
@@ -134,9 +129,6 @@
     <t>Testing the function which gets the file's names with extension .json</t>
   </si>
   <si>
-    <t>12/04/2021 05:53 PM</t>
-  </si>
-  <si>
     <t>Test0.json, Test1.json, Test2.json, Test3.json</t>
   </si>
   <si>
@@ -153,6 +145,69 @@
   </si>
   <si>
     <t>getStatisticsFrom1 / getStatisticsFrom1</t>
+  </si>
+  <si>
+    <t>Test Suite 2 - Automated testing of functions degrees and radians + distances (utils)</t>
+  </si>
+  <si>
+    <t>SS-003</t>
+  </si>
+  <si>
+    <t>toDegree</t>
+  </si>
+  <si>
+    <t>Testing the function which converts radians to degrees</t>
+  </si>
+  <si>
+    <t>08/04/2022 02:41 PM</t>
+  </si>
+  <si>
+    <t>07/04/2022 07:52 PM</t>
+  </si>
+  <si>
+    <t>12/04/2022 05:53 PM</t>
+  </si>
+  <si>
+    <t>01/05/2022 11:26 AM</t>
+  </si>
+  <si>
+    <t>It returns a proper degree value</t>
+  </si>
+  <si>
+    <t>SS-004</t>
+  </si>
+  <si>
+    <t>toRadian</t>
+  </si>
+  <si>
+    <t>Testing the function which converts degrees to radians</t>
+  </si>
+  <si>
+    <t>01/05/2022 11:28 AM</t>
+  </si>
+  <si>
+    <t>It returns a proper radian value</t>
+  </si>
+  <si>
+    <t>Test case 3</t>
+  </si>
+  <si>
+    <t>SS-005</t>
+  </si>
+  <si>
+    <t>getDistance</t>
+  </si>
+  <si>
+    <t>Testing the function which gets the distance between two points</t>
+  </si>
+  <si>
+    <t>01/05/2022 11:30 AM</t>
+  </si>
+  <si>
+    <t>({3,4}, {2,2})</t>
+  </si>
+  <si>
+    <t>It returns a proper distance</t>
   </si>
 </sst>
 </file>
@@ -564,12 +619,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -588,6 +637,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -595,7 +650,7 @@
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="23">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -621,6 +676,12 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
@@ -663,7 +724,52 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -708,7 +814,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E823A22D-AEBF-48ED-9EE6-4BAA3280E420}" name="Table1" displayName="Table1" ref="C10:I12" totalsRowShown="0">
   <autoFilter ref="C10:I12" xr:uid="{CBBAEA08-DC56-4B68-8DF5-9A2681C57DD3}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F045B738-BC81-4AB6-A946-596415D46A39}" name="#" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{F045B738-BC81-4AB6-A946-596415D46A39}" name="#" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{E795166C-74FC-459A-AF28-E24B4C06703E}" name="Description"/>
     <tableColumn id="3" xr3:uid="{CD2CBAEA-36D3-4704-B133-871306A74BA7}" name="Test Data"/>
     <tableColumn id="4" xr3:uid="{19AD3074-2DAA-41E5-89A4-89C039D79A2C}" name="Expectations"/>
@@ -724,13 +830,61 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A0630AD4-6082-455E-AA23-092ABE4DD88D}" name="Table15" displayName="Table15" ref="C24:I26" totalsRowShown="0">
   <autoFilter ref="C24:I26" xr:uid="{A0630AD4-6082-455E-AA23-092ABE4DD88D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{29161239-8648-433E-8E7F-327F36E7512F}" name="#" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{29161239-8648-433E-8E7F-327F36E7512F}" name="#" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{BB3C46E8-1FE6-4CF7-96C1-9567CE973A58}" name="Description"/>
     <tableColumn id="3" xr3:uid="{A4D3DB36-599D-4BE5-ABAA-81C0E54D63AD}" name="Test Data"/>
     <tableColumn id="4" xr3:uid="{2C8185FA-9CE4-4187-A130-5B1F09C6E6C0}" name="Expectations"/>
     <tableColumn id="5" xr3:uid="{AC6A0C8E-A9F5-4D9D-AA13-5F6CC6B0DC78}" name="Actual Result"/>
     <tableColumn id="6" xr3:uid="{EFA33CBC-967C-44D7-8BEB-BE684E83353D}" name="Status"/>
     <tableColumn id="7" xr3:uid="{A2BA86E3-F405-4E3C-8227-854AD8392864}" name="Comments"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4CFFC41F-237E-42C1-A61D-402CDB0B7252}" name="Table14" displayName="Table14" ref="C10:I12" totalsRowShown="0">
+  <autoFilter ref="C10:I12" xr:uid="{4CFFC41F-237E-42C1-A61D-402CDB0B7252}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{88C37E71-A9AA-412D-9231-A1499FD9374B}" name="#" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{AAAB42E8-A4E3-409B-9A33-4AE89C0DCAC5}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{47EE7474-BE0A-443E-99DB-40A1FFFF993B}" name="Test Data"/>
+    <tableColumn id="4" xr3:uid="{6F893482-E1D5-4D33-89EE-52F1314E2631}" name="Expectations"/>
+    <tableColumn id="5" xr3:uid="{B2E72B30-E743-481E-9893-B85B9C53399D}" name="Actual Result"/>
+    <tableColumn id="6" xr3:uid="{949B1B6C-8453-4E8A-B578-32381DA24950}" name="Status"/>
+    <tableColumn id="7" xr3:uid="{58929238-92CA-48BE-98F7-2515C1778FC9}" name="Comments"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{658F0611-CEE0-4F73-AC41-B734857EF5F2}" name="Table156" displayName="Table156" ref="C24:I26" totalsRowShown="0">
+  <autoFilter ref="C24:I26" xr:uid="{658F0611-CEE0-4F73-AC41-B734857EF5F2}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{618D5013-43B7-4963-90DA-F6444014720F}" name="#" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{03EE7B55-C292-448A-9BD5-7DDEBEF865CC}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{983F7566-F2C5-459F-BB59-4142D2EC9BC0}" name="Test Data"/>
+    <tableColumn id="4" xr3:uid="{3660FF0A-9BE0-4FDB-A4C4-FA76093EE05F}" name="Expectations"/>
+    <tableColumn id="5" xr3:uid="{D4B34C27-F939-40CE-B342-F815BCA35F97}" name="Actual Result"/>
+    <tableColumn id="6" xr3:uid="{204C8A37-AB3A-4F5A-8C13-C5E8728AA629}" name="Status"/>
+    <tableColumn id="7" xr3:uid="{3A12F478-AC65-4A60-8401-6FFB42A79AED}" name="Comments"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C7E28B0D-D6D5-4B42-B631-CD36DF5CCB0D}" name="Table1567" displayName="Table1567" ref="C39:I41" totalsRowShown="0">
+  <autoFilter ref="C39:I41" xr:uid="{C7E28B0D-D6D5-4B42-B631-CD36DF5CCB0D}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{84AEFF92-DCDD-474F-8399-81CBCF1C0A7C}" name="#" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{83678418-81D3-42A9-8961-BC0890E96DF5}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{E2CAA6DE-CFE4-4595-A7B6-AFA37E377E48}" name="Test Data"/>
+    <tableColumn id="4" xr3:uid="{9B3459D7-B16F-421C-A91E-B452FC2C061D}" name="Expectations"/>
+    <tableColumn id="5" xr3:uid="{D4E33114-CB8A-4098-8E0C-D3C1ED2B2CC2}" name="Actual Result"/>
+    <tableColumn id="6" xr3:uid="{F36503C0-ABAE-42AF-AFA2-A55E30EFA4CB}" name="Status"/>
+    <tableColumn id="7" xr3:uid="{60DD3F36-758C-4112-9A7F-33CA2C9F5FC1}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1035,33 +1189,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E700B86-A081-4DFE-BEA1-995AE76D7104}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="56.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+    <row r="1" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -1069,19 +1223,19 @@
       <c r="E2" s="4"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="29"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="29"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="24" t="s">
@@ -1097,30 +1251,30 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="26"/>
       <c r="C5" s="25" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="G5" s="22"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="26"/>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="32" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="11" t="s">
@@ -1130,23 +1284,23 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="26"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="35"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="12" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" s="20"/>
       <c r="F8" s="20"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="13" t="s">
         <v>9</v>
       </c>
@@ -1169,7 +1323,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="14">
         <v>1</v>
       </c>
@@ -1177,7 +1331,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
@@ -1186,7 +1340,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="15">
         <v>2</v>
       </c>
@@ -1204,10 +1358,10 @@
         <v>17</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="15"/>
       <c r="D15" s="16"/>
       <c r="E15" s="17"/>
@@ -1216,26 +1370,26 @@
       <c r="H15" s="16"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="17" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B17" s="4"/>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="29"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="24" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>3</v>
@@ -1244,31 +1398,31 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="26"/>
       <c r="C19" s="25" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="G19" s="22"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="26"/>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="34" t="s">
-        <v>31</v>
+      <c r="D20" s="32" t="s">
+        <v>29</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>7</v>
@@ -1277,23 +1431,23 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="26"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="35"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="12" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D22" s="20"/>
       <c r="F22" s="20"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" s="13" t="s">
         <v>9</v>
       </c>
@@ -1316,7 +1470,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="C25" s="14">
         <v>1</v>
       </c>
@@ -1324,7 +1478,7 @@
         <v>15</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G25" t="s">
         <v>16</v>
@@ -1333,7 +1487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C26" s="15">
         <v>2</v>
       </c>
@@ -1351,7 +1505,7 @@
         <v>17</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1365,24 +1519,24 @@
     <mergeCell ref="D6:D7"/>
   </mergeCells>
   <conditionalFormatting sqref="C11:I12 C15:I15">
-    <cfRule type="expression" dxfId="13" priority="16">
+    <cfRule type="expression" dxfId="22" priority="16">
       <formula>$H11="BLOCKED"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="17">
+    <cfRule type="expression" dxfId="21" priority="17">
       <formula>$H11="FAILED"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="18">
+    <cfRule type="expression" dxfId="20" priority="18">
       <formula>$H11="PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:I26">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>$H25="BLOCKED"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>$H25="FAILED"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>$H25="PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1407,6 +1561,534 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53447F16-25A1-4016-B446-7485F6597AF3}">
+  <dimension ref="A1:I41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="29"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="20"/>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="14">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="27">
+        <v>0.78539800000000004</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="15">
+        <v>2</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="18"/>
+    </row>
+    <row r="17" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="22"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="20"/>
+      <c r="F22" s="20"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="14">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="27">
+        <v>45</v>
+      </c>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="15">
+        <v>2</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="29"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="29"/>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G34" s="22"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D37" s="20"/>
+      <c r="F37" s="20"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C39" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" t="s">
+        <v>13</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" s="14">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="G40" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="15">
+        <v>2</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="17"/>
+      <c r="F41" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C11:I12 C15:I15">
+    <cfRule type="expression" dxfId="11" priority="7">
+      <formula>$H11="BLOCKED"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="8">
+      <formula>$H11="FAILED"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="9">
+      <formula>$H11="PASSED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:I26">
+    <cfRule type="expression" dxfId="8" priority="4">
+      <formula>$H25="BLOCKED"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="5">
+      <formula>$H25="FAILED"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>$H25="PASSED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40:I41">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$H40="BLOCKED"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$H40="FAILED"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>$H40="PASSED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00DC9D3D-9037-401D-8075-4C577CA5D5CE}">
+          <x14:formula1>
+            <xm:f>'Values for status dropdown'!$A$1:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>H11:H12 H15 H25:H26 H40:H41</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE0BDE1-888B-4CAC-9F38-73808CDC733D}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -1414,19 +2096,19 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>

</xml_diff>